<commit_message>
Added Description in Chapters and Topics
</commit_message>
<xml_diff>
--- a/Sample Docs/Chapters.xlsx
+++ b/Sample Docs/Chapters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vamsi\Desktop\GIT\Resonance\Sample Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2CDEA5-4299-4A5C-AB1F-50F624E179CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39DDB76-8FBD-4305-8488-05EEF6BCED92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>IsRecommended</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA60C42-192B-42B6-8955-A59C8530898C}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,7 +407,7 @@
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,8 +420,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -432,7 +438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>